<commit_message>
add raw clam data back
</commit_message>
<xml_diff>
--- a/data/raw/2024-02-28_profile-data.xlsx
+++ b/data/raw/2024-02-28_profile-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lysbethkoster/Documents/Universiteit/University of Hawai'i/MSc Thesis/Thesis/RQ2/Data Sets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lysbethkoster/Documents/Universiteit/University of Hawai'i/MSc Thesis/Thesis/RQ2/nomilo-fishpond-analysis/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C17E11-F301-F948-A351-8B6D055418F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B61C17-5849-374C-90D5-E7B43DDF6FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{5D9A96BC-2409-7C40-8704-235FD04ADFD9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{5D9A96BC-2409-7C40-8704-235FD04ADFD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Data" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="34">
   <si>
     <t>Nomilo Fishpond Profiles</t>
   </si>
@@ -132,6 +132,18 @@
   <si>
     <t>total_sample_id</t>
   </si>
+  <si>
+    <t>20/02/24</t>
+  </si>
+  <si>
+    <t>30/1/24</t>
+  </si>
+  <si>
+    <t>20/2/24</t>
+  </si>
+  <si>
+    <t>30/01/24</t>
+  </si>
 </sst>
 </file>
 
@@ -161,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +183,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -203,10 +221,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,7 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{687686CF-AC9D-9A4C-A4E4-763C6107FA7C}">
   <dimension ref="A1:L156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -704,14 +720,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="9">
+      <c r="C11" s="6">
         <v>1</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11">
         <v>2</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>7.5</v>
       </c>
     </row>
@@ -727,7 +743,7 @@
       <c r="E12">
         <v>2</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="9">
         <v>7</v>
       </c>
     </row>
@@ -743,7 +759,7 @@
       <c r="E13">
         <v>2</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="9">
         <v>6.5</v>
       </c>
     </row>
@@ -759,7 +775,7 @@
       <c r="E14">
         <v>2</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="9">
         <v>6</v>
       </c>
     </row>
@@ -775,7 +791,7 @@
       <c r="E15">
         <v>2</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="9">
         <v>5.5</v>
       </c>
     </row>
@@ -791,7 +807,7 @@
       <c r="E16">
         <v>2</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="9">
         <v>5</v>
       </c>
     </row>
@@ -807,7 +823,7 @@
       <c r="E17">
         <v>2</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="9">
         <v>4.5</v>
       </c>
     </row>
@@ -823,7 +839,7 @@
       <c r="E18">
         <v>2</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18" s="9">
         <v>4</v>
       </c>
     </row>
@@ -839,7 +855,7 @@
       <c r="E19">
         <v>2</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="9">
         <v>3.5</v>
       </c>
     </row>
@@ -855,7 +871,7 @@
       <c r="E20">
         <v>2</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="9">
         <v>3</v>
       </c>
     </row>
@@ -864,14 +880,14 @@
         <v>20</v>
       </c>
       <c r="B21" s="6"/>
-      <c r="C21" s="9">
+      <c r="C21" s="6">
         <v>1</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <v>2.5</v>
       </c>
     </row>
@@ -887,7 +903,7 @@
       <c r="E22">
         <v>2</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="9">
         <v>2</v>
       </c>
     </row>
@@ -903,7 +919,7 @@
       <c r="E23">
         <v>2</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="9">
         <v>1.5</v>
       </c>
     </row>
@@ -919,7 +935,7 @@
       <c r="E24">
         <v>2</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24" s="9">
         <v>1</v>
       </c>
     </row>
@@ -935,7 +951,7 @@
       <c r="E25">
         <v>2</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -1024,7 +1040,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="6"/>
-      <c r="C31" s="9">
+      <c r="C31" s="6">
         <v>1</v>
       </c>
       <c r="D31" s="5"/>
@@ -1207,7 +1223,7 @@
       <c r="E42">
         <v>2</v>
       </c>
-      <c r="F42" s="10">
+      <c r="F42" s="9">
         <v>7.5</v>
       </c>
     </row>
@@ -1223,7 +1239,7 @@
       <c r="E43">
         <v>2</v>
       </c>
-      <c r="F43" s="10">
+      <c r="F43" s="9">
         <v>7</v>
       </c>
     </row>
@@ -1239,7 +1255,7 @@
       <c r="E44">
         <v>2</v>
       </c>
-      <c r="F44" s="10">
+      <c r="F44" s="9">
         <v>6.5</v>
       </c>
     </row>
@@ -1253,7 +1269,7 @@
       <c r="E45">
         <v>2</v>
       </c>
-      <c r="F45" s="10">
+      <c r="F45" s="9">
         <v>6</v>
       </c>
     </row>
@@ -1267,7 +1283,7 @@
       <c r="E46">
         <v>2</v>
       </c>
-      <c r="F46" s="10">
+      <c r="F46" s="9">
         <v>5.5</v>
       </c>
     </row>
@@ -1281,7 +1297,7 @@
       <c r="E47">
         <v>2</v>
       </c>
-      <c r="F47" s="10">
+      <c r="F47" s="9">
         <v>5</v>
       </c>
     </row>
@@ -1295,7 +1311,7 @@
       <c r="E48">
         <v>2</v>
       </c>
-      <c r="F48" s="10">
+      <c r="F48" s="9">
         <v>4.5</v>
       </c>
     </row>
@@ -1309,7 +1325,7 @@
       <c r="E49">
         <v>2</v>
       </c>
-      <c r="F49" s="10">
+      <c r="F49" s="9">
         <v>4</v>
       </c>
     </row>
@@ -1323,7 +1339,7 @@
       <c r="E50">
         <v>2</v>
       </c>
-      <c r="F50" s="10">
+      <c r="F50" s="9">
         <v>3.5</v>
       </c>
     </row>
@@ -1337,7 +1353,7 @@
       <c r="E51">
         <v>2</v>
       </c>
-      <c r="F51" s="10">
+      <c r="F51" s="9">
         <v>3</v>
       </c>
     </row>
@@ -1351,7 +1367,7 @@
       <c r="E52">
         <v>2</v>
       </c>
-      <c r="F52" s="10">
+      <c r="F52" s="9">
         <v>2.5</v>
       </c>
     </row>
@@ -1365,7 +1381,7 @@
       <c r="E53">
         <v>2</v>
       </c>
-      <c r="F53" s="10">
+      <c r="F53" s="9">
         <v>2</v>
       </c>
     </row>
@@ -1379,7 +1395,7 @@
       <c r="E54">
         <v>2</v>
       </c>
-      <c r="F54" s="10">
+      <c r="F54" s="9">
         <v>1.5</v>
       </c>
     </row>
@@ -1393,7 +1409,7 @@
       <c r="E55">
         <v>2</v>
       </c>
-      <c r="F55" s="10">
+      <c r="F55" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1407,7 +1423,7 @@
       <c r="E56">
         <v>2</v>
       </c>
-      <c r="F56" s="10">
+      <c r="F56" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -1516,10 +1532,10 @@
       <c r="C64" s="6">
         <v>3</v>
       </c>
-      <c r="E64" s="10">
-        <v>1</v>
-      </c>
-      <c r="F64" s="10">
+      <c r="E64" s="9">
+        <v>1</v>
+      </c>
+      <c r="F64" s="9">
         <v>4.5</v>
       </c>
     </row>
@@ -1530,10 +1546,10 @@
       <c r="C65" s="6">
         <v>3</v>
       </c>
-      <c r="E65" s="10">
-        <v>1</v>
-      </c>
-      <c r="F65" s="10">
+      <c r="E65" s="9">
+        <v>1</v>
+      </c>
+      <c r="F65" s="9">
         <v>4</v>
       </c>
     </row>
@@ -1544,10 +1560,10 @@
       <c r="C66" s="6">
         <v>3</v>
       </c>
-      <c r="E66" s="10">
-        <v>1</v>
-      </c>
-      <c r="F66" s="10">
+      <c r="E66" s="9">
+        <v>1</v>
+      </c>
+      <c r="F66" s="9">
         <v>3.5</v>
       </c>
     </row>
@@ -1558,10 +1574,10 @@
       <c r="C67" s="6">
         <v>3</v>
       </c>
-      <c r="E67" s="10">
-        <v>1</v>
-      </c>
-      <c r="F67" s="10">
+      <c r="E67" s="9">
+        <v>1</v>
+      </c>
+      <c r="F67" s="9">
         <v>3</v>
       </c>
     </row>
@@ -1572,10 +1588,10 @@
       <c r="C68" s="6">
         <v>3</v>
       </c>
-      <c r="E68" s="10">
-        <v>1</v>
-      </c>
-      <c r="F68" s="10">
+      <c r="E68" s="9">
+        <v>1</v>
+      </c>
+      <c r="F68" s="9">
         <v>2.5</v>
       </c>
     </row>
@@ -1586,10 +1602,10 @@
       <c r="C69" s="6">
         <v>3</v>
       </c>
-      <c r="E69" s="10">
-        <v>1</v>
-      </c>
-      <c r="F69" s="10">
+      <c r="E69" s="9">
+        <v>1</v>
+      </c>
+      <c r="F69" s="9">
         <v>2</v>
       </c>
     </row>
@@ -1600,10 +1616,10 @@
       <c r="C70" s="6">
         <v>3</v>
       </c>
-      <c r="E70" s="10">
-        <v>1</v>
-      </c>
-      <c r="F70" s="10">
+      <c r="E70" s="9">
+        <v>1</v>
+      </c>
+      <c r="F70" s="9">
         <v>1.5</v>
       </c>
     </row>
@@ -1614,10 +1630,10 @@
       <c r="C71" s="6">
         <v>3</v>
       </c>
-      <c r="E71" s="10">
-        <v>1</v>
-      </c>
-      <c r="F71" s="10">
+      <c r="E71" s="9">
+        <v>1</v>
+      </c>
+      <c r="F71" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1628,10 +1644,10 @@
       <c r="C72" s="6">
         <v>3</v>
       </c>
-      <c r="E72" s="10">
-        <v>1</v>
-      </c>
-      <c r="F72" s="10">
+      <c r="E72" s="9">
+        <v>1</v>
+      </c>
+      <c r="F72" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -1642,10 +1658,10 @@
       <c r="C73" s="6">
         <v>3</v>
       </c>
-      <c r="E73" s="10">
-        <v>2</v>
-      </c>
-      <c r="F73" s="10">
+      <c r="E73" s="9">
+        <v>2</v>
+      </c>
+      <c r="F73" s="9">
         <v>7.5</v>
       </c>
     </row>
@@ -1656,10 +1672,10 @@
       <c r="C74" s="6">
         <v>3</v>
       </c>
-      <c r="E74" s="10">
-        <v>2</v>
-      </c>
-      <c r="F74" s="10">
+      <c r="E74" s="9">
+        <v>2</v>
+      </c>
+      <c r="F74" s="9">
         <v>7</v>
       </c>
     </row>
@@ -1670,10 +1686,10 @@
       <c r="C75" s="6">
         <v>3</v>
       </c>
-      <c r="E75" s="10">
-        <v>2</v>
-      </c>
-      <c r="F75" s="10">
+      <c r="E75" s="9">
+        <v>2</v>
+      </c>
+      <c r="F75" s="9">
         <v>6.5</v>
       </c>
     </row>
@@ -1684,10 +1700,10 @@
       <c r="C76" s="6">
         <v>3</v>
       </c>
-      <c r="E76" s="10">
-        <v>2</v>
-      </c>
-      <c r="F76" s="10">
+      <c r="E76" s="9">
+        <v>2</v>
+      </c>
+      <c r="F76" s="9">
         <v>6</v>
       </c>
     </row>
@@ -1698,10 +1714,10 @@
       <c r="C77" s="6">
         <v>3</v>
       </c>
-      <c r="E77" s="10">
-        <v>2</v>
-      </c>
-      <c r="F77" s="10">
+      <c r="E77" s="9">
+        <v>2</v>
+      </c>
+      <c r="F77" s="9">
         <v>5.5</v>
       </c>
     </row>
@@ -1712,10 +1728,10 @@
       <c r="C78" s="6">
         <v>3</v>
       </c>
-      <c r="E78" s="10">
-        <v>2</v>
-      </c>
-      <c r="F78" s="10">
+      <c r="E78" s="9">
+        <v>2</v>
+      </c>
+      <c r="F78" s="9">
         <v>5</v>
       </c>
     </row>
@@ -1726,10 +1742,10 @@
       <c r="C79" s="6">
         <v>3</v>
       </c>
-      <c r="E79" s="10">
-        <v>2</v>
-      </c>
-      <c r="F79" s="10">
+      <c r="E79" s="9">
+        <v>2</v>
+      </c>
+      <c r="F79" s="9">
         <v>4.5</v>
       </c>
     </row>
@@ -1740,10 +1756,10 @@
       <c r="C80" s="6">
         <v>3</v>
       </c>
-      <c r="E80" s="10">
-        <v>2</v>
-      </c>
-      <c r="F80" s="10">
+      <c r="E80" s="9">
+        <v>2</v>
+      </c>
+      <c r="F80" s="9">
         <v>4</v>
       </c>
     </row>
@@ -1754,10 +1770,10 @@
       <c r="C81" s="6">
         <v>3</v>
       </c>
-      <c r="E81" s="10">
-        <v>2</v>
-      </c>
-      <c r="F81" s="10">
+      <c r="E81" s="9">
+        <v>2</v>
+      </c>
+      <c r="F81" s="9">
         <v>3.5</v>
       </c>
     </row>
@@ -1768,10 +1784,10 @@
       <c r="C82" s="6">
         <v>3</v>
       </c>
-      <c r="E82" s="10">
-        <v>2</v>
-      </c>
-      <c r="F82" s="10">
+      <c r="E82" s="9">
+        <v>2</v>
+      </c>
+      <c r="F82" s="9">
         <v>3</v>
       </c>
     </row>
@@ -1782,10 +1798,10 @@
       <c r="C83" s="6">
         <v>3</v>
       </c>
-      <c r="E83" s="10">
-        <v>2</v>
-      </c>
-      <c r="F83" s="10">
+      <c r="E83" s="9">
+        <v>2</v>
+      </c>
+      <c r="F83" s="9">
         <v>2.5</v>
       </c>
     </row>
@@ -1796,10 +1812,10 @@
       <c r="C84" s="6">
         <v>3</v>
       </c>
-      <c r="E84" s="10">
-        <v>2</v>
-      </c>
-      <c r="F84" s="10">
+      <c r="E84" s="9">
+        <v>2</v>
+      </c>
+      <c r="F84" s="9">
         <v>2</v>
       </c>
     </row>
@@ -1810,10 +1826,10 @@
       <c r="C85" s="6">
         <v>3</v>
       </c>
-      <c r="E85" s="10">
-        <v>2</v>
-      </c>
-      <c r="F85" s="10">
+      <c r="E85" s="9">
+        <v>2</v>
+      </c>
+      <c r="F85" s="9">
         <v>1.5</v>
       </c>
     </row>
@@ -1824,10 +1840,10 @@
       <c r="C86" s="6">
         <v>3</v>
       </c>
-      <c r="E86" s="10">
-        <v>2</v>
-      </c>
-      <c r="F86" s="10">
+      <c r="E86" s="9">
+        <v>2</v>
+      </c>
+      <c r="F86" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1838,10 +1854,10 @@
       <c r="C87" s="6">
         <v>3</v>
       </c>
-      <c r="E87" s="10">
-        <v>2</v>
-      </c>
-      <c r="F87" s="10">
+      <c r="E87" s="9">
+        <v>2</v>
+      </c>
+      <c r="F87" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -1852,10 +1868,10 @@
       <c r="C88" s="6">
         <v>3</v>
       </c>
-      <c r="E88" s="10">
-        <v>3</v>
-      </c>
-      <c r="F88" s="10">
+      <c r="E88" s="9">
+        <v>3</v>
+      </c>
+      <c r="F88" s="9">
         <v>2.5</v>
       </c>
     </row>
@@ -1866,10 +1882,10 @@
       <c r="C89" s="6">
         <v>3</v>
       </c>
-      <c r="E89" s="10">
-        <v>3</v>
-      </c>
-      <c r="F89" s="10">
+      <c r="E89" s="9">
+        <v>3</v>
+      </c>
+      <c r="F89" s="9">
         <v>2</v>
       </c>
     </row>
@@ -1880,10 +1896,10 @@
       <c r="C90" s="6">
         <v>3</v>
       </c>
-      <c r="E90" s="10">
-        <v>3</v>
-      </c>
-      <c r="F90" s="10">
+      <c r="E90" s="9">
+        <v>3</v>
+      </c>
+      <c r="F90" s="9">
         <v>1.5</v>
       </c>
     </row>
@@ -1894,10 +1910,10 @@
       <c r="C91" s="6">
         <v>3</v>
       </c>
-      <c r="E91" s="10">
-        <v>3</v>
-      </c>
-      <c r="F91" s="10">
+      <c r="E91" s="9">
+        <v>3</v>
+      </c>
+      <c r="F91" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1908,10 +1924,10 @@
       <c r="C92" s="6">
         <v>3</v>
       </c>
-      <c r="E92" s="10">
-        <v>3</v>
-      </c>
-      <c r="F92" s="10">
+      <c r="E92" s="9">
+        <v>3</v>
+      </c>
+      <c r="F92" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -1922,10 +1938,10 @@
       <c r="C93" s="6">
         <v>3</v>
       </c>
-      <c r="E93" s="10">
-        <v>4</v>
-      </c>
-      <c r="F93" s="10">
+      <c r="E93" s="9">
+        <v>4</v>
+      </c>
+      <c r="F93" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1936,10 +1952,10 @@
       <c r="C94" s="6">
         <v>3</v>
       </c>
-      <c r="E94" s="10">
-        <v>4</v>
-      </c>
-      <c r="F94" s="10">
+      <c r="E94" s="9">
+        <v>4</v>
+      </c>
+      <c r="F94" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -1950,10 +1966,10 @@
       <c r="C95" s="6">
         <v>4</v>
       </c>
-      <c r="E95" s="10">
-        <v>1</v>
-      </c>
-      <c r="F95" s="10">
+      <c r="E95" s="9">
+        <v>1</v>
+      </c>
+      <c r="F95" s="9">
         <v>4.5</v>
       </c>
     </row>
@@ -1964,10 +1980,10 @@
       <c r="C96" s="6">
         <v>4</v>
       </c>
-      <c r="E96" s="10">
-        <v>1</v>
-      </c>
-      <c r="F96" s="10">
+      <c r="E96" s="9">
+        <v>1</v>
+      </c>
+      <c r="F96" s="9">
         <v>4</v>
       </c>
     </row>
@@ -1978,10 +1994,10 @@
       <c r="C97" s="6">
         <v>4</v>
       </c>
-      <c r="E97" s="10">
-        <v>1</v>
-      </c>
-      <c r="F97" s="10">
+      <c r="E97" s="9">
+        <v>1</v>
+      </c>
+      <c r="F97" s="9">
         <v>3.5</v>
       </c>
     </row>
@@ -1992,10 +2008,10 @@
       <c r="C98" s="6">
         <v>4</v>
       </c>
-      <c r="E98" s="10">
-        <v>1</v>
-      </c>
-      <c r="F98" s="10">
+      <c r="E98" s="9">
+        <v>1</v>
+      </c>
+      <c r="F98" s="9">
         <v>3</v>
       </c>
     </row>
@@ -2006,10 +2022,10 @@
       <c r="C99" s="6">
         <v>4</v>
       </c>
-      <c r="E99" s="10">
-        <v>1</v>
-      </c>
-      <c r="F99" s="10">
+      <c r="E99" s="9">
+        <v>1</v>
+      </c>
+      <c r="F99" s="9">
         <v>2.5</v>
       </c>
     </row>
@@ -2020,10 +2036,10 @@
       <c r="C100" s="6">
         <v>4</v>
       </c>
-      <c r="E100" s="10">
-        <v>1</v>
-      </c>
-      <c r="F100" s="10">
+      <c r="E100" s="9">
+        <v>1</v>
+      </c>
+      <c r="F100" s="9">
         <v>2</v>
       </c>
     </row>
@@ -2034,10 +2050,10 @@
       <c r="C101" s="6">
         <v>4</v>
       </c>
-      <c r="E101" s="10">
-        <v>1</v>
-      </c>
-      <c r="F101" s="10">
+      <c r="E101" s="9">
+        <v>1</v>
+      </c>
+      <c r="F101" s="9">
         <v>1.5</v>
       </c>
     </row>
@@ -2048,10 +2064,10 @@
       <c r="C102" s="6">
         <v>4</v>
       </c>
-      <c r="E102" s="10">
-        <v>1</v>
-      </c>
-      <c r="F102" s="10">
+      <c r="E102" s="9">
+        <v>1</v>
+      </c>
+      <c r="F102" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2062,10 +2078,10 @@
       <c r="C103" s="6">
         <v>4</v>
       </c>
-      <c r="E103" s="10">
-        <v>1</v>
-      </c>
-      <c r="F103" s="10">
+      <c r="E103" s="9">
+        <v>1</v>
+      </c>
+      <c r="F103" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -2076,10 +2092,10 @@
       <c r="C104" s="6">
         <v>4</v>
       </c>
-      <c r="E104" s="10">
-        <v>2</v>
-      </c>
-      <c r="F104" s="10">
+      <c r="E104" s="9">
+        <v>2</v>
+      </c>
+      <c r="F104" s="9">
         <v>7.5</v>
       </c>
     </row>
@@ -2090,10 +2106,10 @@
       <c r="C105" s="6">
         <v>4</v>
       </c>
-      <c r="E105" s="10">
-        <v>2</v>
-      </c>
-      <c r="F105" s="10">
+      <c r="E105" s="9">
+        <v>2</v>
+      </c>
+      <c r="F105" s="9">
         <v>7</v>
       </c>
     </row>
@@ -2104,10 +2120,10 @@
       <c r="C106" s="6">
         <v>4</v>
       </c>
-      <c r="E106" s="10">
-        <v>2</v>
-      </c>
-      <c r="F106" s="10">
+      <c r="E106" s="9">
+        <v>2</v>
+      </c>
+      <c r="F106" s="9">
         <v>6.5</v>
       </c>
     </row>
@@ -2118,10 +2134,10 @@
       <c r="C107" s="6">
         <v>4</v>
       </c>
-      <c r="E107" s="10">
-        <v>2</v>
-      </c>
-      <c r="F107" s="10">
+      <c r="E107" s="9">
+        <v>2</v>
+      </c>
+      <c r="F107" s="9">
         <v>6</v>
       </c>
     </row>
@@ -2132,10 +2148,10 @@
       <c r="C108" s="6">
         <v>4</v>
       </c>
-      <c r="E108" s="10">
-        <v>2</v>
-      </c>
-      <c r="F108" s="10">
+      <c r="E108" s="9">
+        <v>2</v>
+      </c>
+      <c r="F108" s="9">
         <v>5.5</v>
       </c>
     </row>
@@ -2146,10 +2162,10 @@
       <c r="C109" s="6">
         <v>4</v>
       </c>
-      <c r="E109" s="10">
-        <v>2</v>
-      </c>
-      <c r="F109" s="10">
+      <c r="E109" s="9">
+        <v>2</v>
+      </c>
+      <c r="F109" s="9">
         <v>5</v>
       </c>
     </row>
@@ -2160,10 +2176,10 @@
       <c r="C110" s="6">
         <v>4</v>
       </c>
-      <c r="E110" s="10">
-        <v>2</v>
-      </c>
-      <c r="F110" s="10">
+      <c r="E110" s="9">
+        <v>2</v>
+      </c>
+      <c r="F110" s="9">
         <v>4.5</v>
       </c>
     </row>
@@ -2174,10 +2190,10 @@
       <c r="C111" s="6">
         <v>4</v>
       </c>
-      <c r="E111" s="10">
-        <v>2</v>
-      </c>
-      <c r="F111" s="10">
+      <c r="E111" s="9">
+        <v>2</v>
+      </c>
+      <c r="F111" s="9">
         <v>4</v>
       </c>
     </row>
@@ -2188,10 +2204,10 @@
       <c r="C112" s="6">
         <v>4</v>
       </c>
-      <c r="E112" s="10">
-        <v>2</v>
-      </c>
-      <c r="F112" s="10">
+      <c r="E112" s="9">
+        <v>2</v>
+      </c>
+      <c r="F112" s="9">
         <v>3.5</v>
       </c>
     </row>
@@ -2202,10 +2218,10 @@
       <c r="C113" s="6">
         <v>4</v>
       </c>
-      <c r="E113" s="10">
-        <v>2</v>
-      </c>
-      <c r="F113" s="10">
+      <c r="E113" s="9">
+        <v>2</v>
+      </c>
+      <c r="F113" s="9">
         <v>3</v>
       </c>
     </row>
@@ -2216,10 +2232,10 @@
       <c r="C114" s="6">
         <v>4</v>
       </c>
-      <c r="E114" s="10">
-        <v>2</v>
-      </c>
-      <c r="F114" s="10">
+      <c r="E114" s="9">
+        <v>2</v>
+      </c>
+      <c r="F114" s="9">
         <v>2.5</v>
       </c>
     </row>
@@ -2230,10 +2246,10 @@
       <c r="C115" s="6">
         <v>4</v>
       </c>
-      <c r="E115" s="10">
-        <v>2</v>
-      </c>
-      <c r="F115" s="10">
+      <c r="E115" s="9">
+        <v>2</v>
+      </c>
+      <c r="F115" s="9">
         <v>2</v>
       </c>
     </row>
@@ -2244,10 +2260,10 @@
       <c r="C116" s="6">
         <v>4</v>
       </c>
-      <c r="E116" s="10">
-        <v>2</v>
-      </c>
-      <c r="F116" s="10">
+      <c r="E116" s="9">
+        <v>2</v>
+      </c>
+      <c r="F116" s="9">
         <v>1.5</v>
       </c>
     </row>
@@ -2258,10 +2274,10 @@
       <c r="C117" s="6">
         <v>4</v>
       </c>
-      <c r="E117" s="10">
-        <v>2</v>
-      </c>
-      <c r="F117" s="10">
+      <c r="E117" s="9">
+        <v>2</v>
+      </c>
+      <c r="F117" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2272,10 +2288,10 @@
       <c r="C118" s="6">
         <v>4</v>
       </c>
-      <c r="E118" s="10">
-        <v>2</v>
-      </c>
-      <c r="F118" s="10">
+      <c r="E118" s="9">
+        <v>2</v>
+      </c>
+      <c r="F118" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -2286,10 +2302,10 @@
       <c r="C119" s="6">
         <v>4</v>
       </c>
-      <c r="E119" s="10">
-        <v>3</v>
-      </c>
-      <c r="F119" s="10">
+      <c r="E119" s="9">
+        <v>3</v>
+      </c>
+      <c r="F119" s="9">
         <v>2.5</v>
       </c>
     </row>
@@ -2300,10 +2316,10 @@
       <c r="C120" s="6">
         <v>4</v>
       </c>
-      <c r="E120" s="10">
-        <v>3</v>
-      </c>
-      <c r="F120" s="10">
+      <c r="E120" s="9">
+        <v>3</v>
+      </c>
+      <c r="F120" s="9">
         <v>2</v>
       </c>
     </row>
@@ -2314,10 +2330,10 @@
       <c r="C121" s="6">
         <v>4</v>
       </c>
-      <c r="E121" s="10">
-        <v>3</v>
-      </c>
-      <c r="F121" s="10">
+      <c r="E121" s="9">
+        <v>3</v>
+      </c>
+      <c r="F121" s="9">
         <v>1.5</v>
       </c>
     </row>
@@ -2328,10 +2344,10 @@
       <c r="C122" s="6">
         <v>4</v>
       </c>
-      <c r="E122" s="10">
-        <v>3</v>
-      </c>
-      <c r="F122" s="10">
+      <c r="E122" s="9">
+        <v>3</v>
+      </c>
+      <c r="F122" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2342,10 +2358,10 @@
       <c r="C123" s="6">
         <v>4</v>
       </c>
-      <c r="E123" s="10">
-        <v>3</v>
-      </c>
-      <c r="F123" s="10">
+      <c r="E123" s="9">
+        <v>3</v>
+      </c>
+      <c r="F123" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -2356,10 +2372,10 @@
       <c r="C124" s="6">
         <v>4</v>
       </c>
-      <c r="E124" s="10">
-        <v>4</v>
-      </c>
-      <c r="F124" s="10">
+      <c r="E124" s="9">
+        <v>4</v>
+      </c>
+      <c r="F124" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2370,10 +2386,10 @@
       <c r="C125" s="6">
         <v>4</v>
       </c>
-      <c r="E125" s="10">
-        <v>4</v>
-      </c>
-      <c r="F125" s="10">
+      <c r="E125" s="9">
+        <v>4</v>
+      </c>
+      <c r="F125" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -2384,10 +2400,10 @@
       <c r="C126" s="6">
         <v>5</v>
       </c>
-      <c r="E126" s="10">
-        <v>1</v>
-      </c>
-      <c r="F126" s="10">
+      <c r="E126" s="9">
+        <v>1</v>
+      </c>
+      <c r="F126" s="9">
         <v>4.5</v>
       </c>
     </row>
@@ -2398,10 +2414,10 @@
       <c r="C127" s="6">
         <v>5</v>
       </c>
-      <c r="E127" s="10">
-        <v>1</v>
-      </c>
-      <c r="F127" s="10">
+      <c r="E127" s="9">
+        <v>1</v>
+      </c>
+      <c r="F127" s="9">
         <v>4</v>
       </c>
     </row>
@@ -2412,10 +2428,10 @@
       <c r="C128" s="6">
         <v>5</v>
       </c>
-      <c r="E128" s="10">
-        <v>1</v>
-      </c>
-      <c r="F128" s="10">
+      <c r="E128" s="9">
+        <v>1</v>
+      </c>
+      <c r="F128" s="9">
         <v>3.5</v>
       </c>
     </row>
@@ -2426,10 +2442,10 @@
       <c r="C129" s="6">
         <v>5</v>
       </c>
-      <c r="E129" s="10">
-        <v>1</v>
-      </c>
-      <c r="F129" s="10">
+      <c r="E129" s="9">
+        <v>1</v>
+      </c>
+      <c r="F129" s="9">
         <v>3</v>
       </c>
     </row>
@@ -2440,10 +2456,10 @@
       <c r="C130" s="6">
         <v>5</v>
       </c>
-      <c r="E130" s="10">
-        <v>1</v>
-      </c>
-      <c r="F130" s="10">
+      <c r="E130" s="9">
+        <v>1</v>
+      </c>
+      <c r="F130" s="9">
         <v>2.5</v>
       </c>
     </row>
@@ -2454,10 +2470,10 @@
       <c r="C131" s="6">
         <v>5</v>
       </c>
-      <c r="E131" s="10">
-        <v>1</v>
-      </c>
-      <c r="F131" s="10">
+      <c r="E131" s="9">
+        <v>1</v>
+      </c>
+      <c r="F131" s="9">
         <v>2</v>
       </c>
     </row>
@@ -2468,10 +2484,10 @@
       <c r="C132" s="6">
         <v>5</v>
       </c>
-      <c r="E132" s="10">
-        <v>1</v>
-      </c>
-      <c r="F132" s="10">
+      <c r="E132" s="9">
+        <v>1</v>
+      </c>
+      <c r="F132" s="9">
         <v>1.5</v>
       </c>
     </row>
@@ -2482,10 +2498,10 @@
       <c r="C133" s="6">
         <v>5</v>
       </c>
-      <c r="E133" s="10">
-        <v>1</v>
-      </c>
-      <c r="F133" s="10">
+      <c r="E133" s="9">
+        <v>1</v>
+      </c>
+      <c r="F133" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2496,10 +2512,10 @@
       <c r="C134" s="6">
         <v>5</v>
       </c>
-      <c r="E134" s="10">
-        <v>1</v>
-      </c>
-      <c r="F134" s="10">
+      <c r="E134" s="9">
+        <v>1</v>
+      </c>
+      <c r="F134" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -2510,10 +2526,10 @@
       <c r="C135" s="6">
         <v>5</v>
       </c>
-      <c r="E135" s="10">
-        <v>2</v>
-      </c>
-      <c r="F135" s="10">
+      <c r="E135" s="9">
+        <v>2</v>
+      </c>
+      <c r="F135" s="9">
         <v>7.5</v>
       </c>
     </row>
@@ -2524,10 +2540,10 @@
       <c r="C136" s="6">
         <v>5</v>
       </c>
-      <c r="E136" s="10">
-        <v>2</v>
-      </c>
-      <c r="F136" s="10">
+      <c r="E136" s="9">
+        <v>2</v>
+      </c>
+      <c r="F136" s="9">
         <v>7</v>
       </c>
     </row>
@@ -2538,10 +2554,10 @@
       <c r="C137" s="6">
         <v>5</v>
       </c>
-      <c r="E137" s="10">
-        <v>2</v>
-      </c>
-      <c r="F137" s="10">
+      <c r="E137" s="9">
+        <v>2</v>
+      </c>
+      <c r="F137" s="9">
         <v>6.5</v>
       </c>
     </row>
@@ -2552,10 +2568,10 @@
       <c r="C138" s="6">
         <v>5</v>
       </c>
-      <c r="E138" s="10">
-        <v>2</v>
-      </c>
-      <c r="F138" s="10">
+      <c r="E138" s="9">
+        <v>2</v>
+      </c>
+      <c r="F138" s="9">
         <v>6</v>
       </c>
     </row>
@@ -2566,10 +2582,10 @@
       <c r="C139" s="6">
         <v>5</v>
       </c>
-      <c r="E139" s="10">
-        <v>2</v>
-      </c>
-      <c r="F139" s="10">
+      <c r="E139" s="9">
+        <v>2</v>
+      </c>
+      <c r="F139" s="9">
         <v>5.5</v>
       </c>
     </row>
@@ -2580,10 +2596,10 @@
       <c r="C140" s="6">
         <v>5</v>
       </c>
-      <c r="E140" s="10">
-        <v>2</v>
-      </c>
-      <c r="F140" s="10">
+      <c r="E140" s="9">
+        <v>2</v>
+      </c>
+      <c r="F140" s="9">
         <v>5</v>
       </c>
     </row>
@@ -2594,10 +2610,10 @@
       <c r="C141" s="6">
         <v>5</v>
       </c>
-      <c r="E141" s="10">
-        <v>2</v>
-      </c>
-      <c r="F141" s="10">
+      <c r="E141" s="9">
+        <v>2</v>
+      </c>
+      <c r="F141" s="9">
         <v>4.5</v>
       </c>
     </row>
@@ -2608,10 +2624,10 @@
       <c r="C142" s="6">
         <v>5</v>
       </c>
-      <c r="E142" s="10">
-        <v>2</v>
-      </c>
-      <c r="F142" s="10">
+      <c r="E142" s="9">
+        <v>2</v>
+      </c>
+      <c r="F142" s="9">
         <v>4</v>
       </c>
     </row>
@@ -2622,10 +2638,10 @@
       <c r="C143" s="6">
         <v>5</v>
       </c>
-      <c r="E143" s="10">
-        <v>2</v>
-      </c>
-      <c r="F143" s="10">
+      <c r="E143" s="9">
+        <v>2</v>
+      </c>
+      <c r="F143" s="9">
         <v>3.5</v>
       </c>
     </row>
@@ -2636,10 +2652,10 @@
       <c r="C144" s="6">
         <v>5</v>
       </c>
-      <c r="E144" s="10">
-        <v>2</v>
-      </c>
-      <c r="F144" s="10">
+      <c r="E144" s="9">
+        <v>2</v>
+      </c>
+      <c r="F144" s="9">
         <v>3</v>
       </c>
     </row>
@@ -2650,10 +2666,10 @@
       <c r="C145" s="6">
         <v>5</v>
       </c>
-      <c r="E145" s="10">
-        <v>2</v>
-      </c>
-      <c r="F145" s="10">
+      <c r="E145" s="9">
+        <v>2</v>
+      </c>
+      <c r="F145" s="9">
         <v>2.5</v>
       </c>
     </row>
@@ -2664,10 +2680,10 @@
       <c r="C146" s="6">
         <v>5</v>
       </c>
-      <c r="E146" s="10">
-        <v>2</v>
-      </c>
-      <c r="F146" s="10">
+      <c r="E146" s="9">
+        <v>2</v>
+      </c>
+      <c r="F146" s="9">
         <v>2</v>
       </c>
     </row>
@@ -2678,10 +2694,10 @@
       <c r="C147" s="6">
         <v>5</v>
       </c>
-      <c r="E147" s="10">
-        <v>2</v>
-      </c>
-      <c r="F147" s="10">
+      <c r="E147" s="9">
+        <v>2</v>
+      </c>
+      <c r="F147" s="9">
         <v>1.5</v>
       </c>
     </row>
@@ -2692,10 +2708,10 @@
       <c r="C148" s="6">
         <v>5</v>
       </c>
-      <c r="E148" s="10">
-        <v>2</v>
-      </c>
-      <c r="F148" s="10">
+      <c r="E148" s="9">
+        <v>2</v>
+      </c>
+      <c r="F148" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2706,10 +2722,10 @@
       <c r="C149" s="6">
         <v>5</v>
       </c>
-      <c r="E149" s="10">
-        <v>2</v>
-      </c>
-      <c r="F149" s="10">
+      <c r="E149" s="9">
+        <v>2</v>
+      </c>
+      <c r="F149" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -2720,10 +2736,10 @@
       <c r="C150" s="6">
         <v>5</v>
       </c>
-      <c r="E150" s="10">
-        <v>3</v>
-      </c>
-      <c r="F150" s="10">
+      <c r="E150" s="9">
+        <v>3</v>
+      </c>
+      <c r="F150" s="9">
         <v>2.5</v>
       </c>
     </row>
@@ -2734,10 +2750,10 @@
       <c r="C151" s="6">
         <v>5</v>
       </c>
-      <c r="E151" s="10">
-        <v>3</v>
-      </c>
-      <c r="F151" s="10">
+      <c r="E151" s="9">
+        <v>3</v>
+      </c>
+      <c r="F151" s="9">
         <v>2</v>
       </c>
     </row>
@@ -2748,10 +2764,10 @@
       <c r="C152" s="6">
         <v>5</v>
       </c>
-      <c r="E152" s="10">
-        <v>3</v>
-      </c>
-      <c r="F152" s="10">
+      <c r="E152" s="9">
+        <v>3</v>
+      </c>
+      <c r="F152" s="9">
         <v>1.5</v>
       </c>
     </row>
@@ -2762,10 +2778,10 @@
       <c r="C153" s="6">
         <v>5</v>
       </c>
-      <c r="E153" s="10">
-        <v>3</v>
-      </c>
-      <c r="F153" s="10">
+      <c r="E153" s="9">
+        <v>3</v>
+      </c>
+      <c r="F153" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2776,10 +2792,10 @@
       <c r="C154" s="6">
         <v>5</v>
       </c>
-      <c r="E154" s="10">
-        <v>3</v>
-      </c>
-      <c r="F154" s="10">
+      <c r="E154" s="9">
+        <v>3</v>
+      </c>
+      <c r="F154" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -2790,10 +2806,10 @@
       <c r="C155" s="6">
         <v>5</v>
       </c>
-      <c r="E155" s="10">
-        <v>4</v>
-      </c>
-      <c r="F155" s="10">
+      <c r="E155" s="9">
+        <v>4</v>
+      </c>
+      <c r="F155" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2804,10 +2820,10 @@
       <c r="C156" s="6">
         <v>5</v>
       </c>
-      <c r="E156" s="10">
-        <v>4</v>
-      </c>
-      <c r="F156" s="10">
+      <c r="E156" s="9">
+        <v>4</v>
+      </c>
+      <c r="F156" s="9">
         <v>0.5</v>
       </c>
     </row>
@@ -2818,10 +2834,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732354D4-6E48-794C-B788-BFDB59E80D13}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A14"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2862,7 +2878,7 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
@@ -3232,6 +3248,15 @@
       <c r="A30">
         <v>4.5</v>
       </c>
+      <c r="B30">
+        <v>24.4</v>
+      </c>
+      <c r="C30">
+        <v>0.5</v>
+      </c>
+      <c r="E30">
+        <v>38.1</v>
+      </c>
       <c r="F30" s="2">
         <v>0.5083333333333333</v>
       </c>
@@ -3267,7 +3292,7 @@
         <v>38.9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -3281,7 +3306,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2.5</v>
       </c>
@@ -3295,7 +3320,7 @@
         <v>39.1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2</v>
       </c>
@@ -3309,7 +3334,7 @@
         <v>39.299999999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1.5</v>
       </c>
@@ -3323,7 +3348,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -3337,7 +3362,7 @@
         <v>39.700000000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.5</v>
       </c>
@@ -3349,6 +3374,332 @@
       </c>
       <c r="E38">
         <v>39.799999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>4.5</v>
+      </c>
+      <c r="B42">
+        <v>25.3</v>
+      </c>
+      <c r="C42">
+        <v>0.51</v>
+      </c>
+      <c r="E42">
+        <v>41.1</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="G42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>25</v>
+      </c>
+      <c r="C43">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="E43">
+        <v>41.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>3.5</v>
+      </c>
+      <c r="B44">
+        <v>25.1</v>
+      </c>
+      <c r="C44">
+        <v>7.5</v>
+      </c>
+      <c r="E44">
+        <v>41.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>25.2</v>
+      </c>
+      <c r="C45">
+        <v>8.5</v>
+      </c>
+      <c r="E45">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2.5</v>
+      </c>
+      <c r="B46">
+        <v>25</v>
+      </c>
+      <c r="C46">
+        <v>8.6</v>
+      </c>
+      <c r="E46">
+        <v>41.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <v>25</v>
+      </c>
+      <c r="C47">
+        <v>8.82</v>
+      </c>
+      <c r="E47">
+        <v>42.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1.5</v>
+      </c>
+      <c r="B48">
+        <v>25</v>
+      </c>
+      <c r="C48">
+        <v>9.39</v>
+      </c>
+      <c r="E48">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>25</v>
+      </c>
+      <c r="C49">
+        <v>9.67</v>
+      </c>
+      <c r="E49">
+        <v>43.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>0.5</v>
+      </c>
+      <c r="B50">
+        <v>25.1</v>
+      </c>
+      <c r="C50">
+        <v>9.58</v>
+      </c>
+      <c r="E50">
+        <v>43.4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
+        <v>22</v>
+      </c>
+      <c r="F53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>4.5</v>
+      </c>
+      <c r="B54">
+        <v>23.2</v>
+      </c>
+      <c r="C54">
+        <v>9</v>
+      </c>
+      <c r="E54">
+        <v>51.8</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0.59375</v>
+      </c>
+      <c r="G54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>4</v>
+      </c>
+      <c r="B55">
+        <v>23.3</v>
+      </c>
+      <c r="C55">
+        <v>9.02</v>
+      </c>
+      <c r="E55">
+        <v>51.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>3.5</v>
+      </c>
+      <c r="B56">
+        <v>23.1</v>
+      </c>
+      <c r="C56">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="E56">
+        <v>51.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>23.1</v>
+      </c>
+      <c r="C57">
+        <v>9.6</v>
+      </c>
+      <c r="E57">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2.5</v>
+      </c>
+      <c r="B58">
+        <v>23.2</v>
+      </c>
+      <c r="C58">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E58">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>2</v>
+      </c>
+      <c r="B59">
+        <v>23.7</v>
+      </c>
+      <c r="C59">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="E59">
+        <v>52.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1.5</v>
+      </c>
+      <c r="B60">
+        <v>23.9</v>
+      </c>
+      <c r="C60">
+        <v>10</v>
+      </c>
+      <c r="E60">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>24</v>
+      </c>
+      <c r="C61">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="E61">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>0.5</v>
+      </c>
+      <c r="B62">
+        <v>24.2</v>
+      </c>
+      <c r="C62">
+        <v>9.9</v>
+      </c>
+      <c r="E62">
+        <v>52.2</v>
       </c>
     </row>
   </sheetData>
@@ -3358,10 +3709,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{835E0945-C303-C54D-A4FE-D6F39A4AF74B}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3823,70 +4174,64 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
         <v>6</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>7</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>22</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>9</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G40" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>7.5</v>
-      </c>
-      <c r="B40">
-        <v>24</v>
-      </c>
-      <c r="C40">
-        <v>4.05</v>
-      </c>
-      <c r="E40">
-        <v>51.4</v>
-      </c>
-      <c r="F40" s="2">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="G40">
-        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="B41">
         <v>24</v>
       </c>
       <c r="C41">
-        <v>4.82</v>
+        <v>4.05</v>
       </c>
       <c r="E41">
-        <v>51.5</v>
+        <v>51.4</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="G41">
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="B42">
         <v>24</v>
       </c>
       <c r="C42">
-        <v>5.22</v>
+        <v>4.82</v>
       </c>
       <c r="E42">
         <v>51.5</v>
@@ -3894,13 +4239,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="B43">
         <v>24</v>
       </c>
       <c r="C43">
-        <v>5.85</v>
+        <v>5.22</v>
       </c>
       <c r="E43">
         <v>51.5</v>
@@ -3908,13 +4253,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="B44">
         <v>24</v>
       </c>
       <c r="C44">
-        <v>5.83</v>
+        <v>5.85</v>
       </c>
       <c r="E44">
         <v>51.5</v>
@@ -3922,13 +4267,13 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="B45">
-        <v>24.2</v>
+        <v>24</v>
       </c>
       <c r="C45">
-        <v>6.87</v>
+        <v>5.83</v>
       </c>
       <c r="E45">
         <v>51.5</v>
@@ -3936,13 +4281,13 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="B46">
-        <v>24.3</v>
+        <v>24.2</v>
       </c>
       <c r="C46">
-        <v>7.4</v>
+        <v>6.87</v>
       </c>
       <c r="E46">
         <v>51.5</v>
@@ -3950,13 +4295,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="B47">
-        <v>24.4</v>
+        <v>24.3</v>
       </c>
       <c r="C47">
-        <v>7.89</v>
+        <v>7.4</v>
       </c>
       <c r="E47">
         <v>51.5</v>
@@ -3964,100 +4309,608 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="B48">
         <v>24.4</v>
       </c>
       <c r="C48">
-        <v>8.19</v>
+        <v>7.89</v>
       </c>
       <c r="E48">
-        <v>51.2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="B49">
         <v>24.4</v>
       </c>
       <c r="C49">
-        <v>8.33</v>
+        <v>8.19</v>
       </c>
       <c r="E49">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="B50">
         <v>24.4</v>
       </c>
       <c r="C50">
-        <v>8.3699999999999992</v>
+        <v>8.33</v>
       </c>
       <c r="E50">
-        <v>50.9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="B51">
         <v>24.4</v>
       </c>
       <c r="C51">
-        <v>8.4700000000000006</v>
+        <v>8.3699999999999992</v>
       </c>
       <c r="E51">
         <v>50.9</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="B52">
         <v>24.4</v>
       </c>
       <c r="C52">
-        <v>8.5299999999999994</v>
+        <v>8.4700000000000006</v>
       </c>
       <c r="E52">
         <v>50.9</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="B53">
         <v>24.4</v>
       </c>
       <c r="C53">
-        <v>8.48</v>
+        <v>8.5299999999999994</v>
       </c>
       <c r="E53">
         <v>50.9</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="B54">
-        <v>24.5</v>
+        <v>24.4</v>
       </c>
       <c r="C54">
-        <v>8.64</v>
+        <v>8.48</v>
       </c>
       <c r="E54">
         <v>50.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>0.5</v>
+      </c>
+      <c r="B55">
+        <v>24.5</v>
+      </c>
+      <c r="C55">
+        <v>8.64</v>
+      </c>
+      <c r="E55">
+        <v>50.9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" t="s">
+        <v>22</v>
+      </c>
+      <c r="F58" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>7.5</v>
+      </c>
+      <c r="B59">
+        <v>25.2</v>
+      </c>
+      <c r="C59">
+        <v>0.34</v>
+      </c>
+      <c r="E59">
+        <v>41.2</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="G59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>7</v>
+      </c>
+      <c r="B60">
+        <v>24.9</v>
+      </c>
+      <c r="C60">
+        <v>1.9</v>
+      </c>
+      <c r="E60">
+        <v>42.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>6.5</v>
+      </c>
+      <c r="B61">
+        <v>24.8</v>
+      </c>
+      <c r="C61">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="E61">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>6</v>
+      </c>
+      <c r="B62">
+        <v>24.8</v>
+      </c>
+      <c r="C62">
+        <v>3.6</v>
+      </c>
+      <c r="E62">
+        <v>42.7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>5.5</v>
+      </c>
+      <c r="B63">
+        <v>24.8</v>
+      </c>
+      <c r="C63">
+        <v>4.43</v>
+      </c>
+      <c r="E63">
+        <v>43.1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>5</v>
+      </c>
+      <c r="B64">
+        <v>24.9</v>
+      </c>
+      <c r="C64">
+        <v>5.49</v>
+      </c>
+      <c r="E64">
+        <v>44.1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>4.5</v>
+      </c>
+      <c r="B65">
+        <v>24.9</v>
+      </c>
+      <c r="C65">
+        <v>6.33</v>
+      </c>
+      <c r="E65">
+        <v>44.8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>4</v>
+      </c>
+      <c r="B66">
+        <v>25</v>
+      </c>
+      <c r="C66">
+        <v>6.74</v>
+      </c>
+      <c r="E66">
+        <v>45.9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>3.5</v>
+      </c>
+      <c r="B67">
+        <v>25</v>
+      </c>
+      <c r="C67">
+        <v>7.51</v>
+      </c>
+      <c r="E67">
+        <v>49.2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>25.1</v>
+      </c>
+      <c r="C68">
+        <v>8.41</v>
+      </c>
+      <c r="E68">
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>2.5</v>
+      </c>
+      <c r="B69">
+        <v>25.2</v>
+      </c>
+      <c r="C69">
+        <v>8.93</v>
+      </c>
+      <c r="E69">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>2</v>
+      </c>
+      <c r="B70">
+        <v>25.3</v>
+      </c>
+      <c r="C70">
+        <v>9.15</v>
+      </c>
+      <c r="E70">
+        <v>51.1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>1.5</v>
+      </c>
+      <c r="B71">
+        <v>25.2</v>
+      </c>
+      <c r="C71">
+        <v>9.35</v>
+      </c>
+      <c r="E71">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72">
+        <v>25.2</v>
+      </c>
+      <c r="C72">
+        <v>9.61</v>
+      </c>
+      <c r="E72">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>0.5</v>
+      </c>
+      <c r="B73">
+        <v>25.3</v>
+      </c>
+      <c r="C73">
+        <v>9.51</v>
+      </c>
+      <c r="E73">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" t="s">
+        <v>22</v>
+      </c>
+      <c r="F76" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>7.5</v>
+      </c>
+      <c r="B77">
+        <v>23.2</v>
+      </c>
+      <c r="C77">
+        <v>0.4</v>
+      </c>
+      <c r="E77">
+        <v>52.2</v>
+      </c>
+      <c r="F77" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>7</v>
+      </c>
+      <c r="B78">
+        <v>23.2</v>
+      </c>
+      <c r="C78">
+        <v>7.5</v>
+      </c>
+      <c r="E78">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>6.5</v>
+      </c>
+      <c r="B79">
+        <v>23.2</v>
+      </c>
+      <c r="C79">
+        <v>8</v>
+      </c>
+      <c r="E79">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>6</v>
+      </c>
+      <c r="B80">
+        <v>23.2</v>
+      </c>
+      <c r="C80">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E80">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>5.5</v>
+      </c>
+      <c r="B81">
+        <v>23.2</v>
+      </c>
+      <c r="C81">
+        <v>8.5</v>
+      </c>
+      <c r="E81">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>5</v>
+      </c>
+      <c r="B82">
+        <v>23.2</v>
+      </c>
+      <c r="C82">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E82">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>4.5</v>
+      </c>
+      <c r="B83">
+        <v>23.1</v>
+      </c>
+      <c r="C83">
+        <v>9</v>
+      </c>
+      <c r="E83">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>4</v>
+      </c>
+      <c r="B84">
+        <v>23</v>
+      </c>
+      <c r="C84">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="E84">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>3.5</v>
+      </c>
+      <c r="B85">
+        <v>23</v>
+      </c>
+      <c r="C85">
+        <v>9.5</v>
+      </c>
+      <c r="E85">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>3</v>
+      </c>
+      <c r="B86">
+        <v>23</v>
+      </c>
+      <c r="C86">
+        <v>9.6</v>
+      </c>
+      <c r="E86">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>2.5</v>
+      </c>
+      <c r="B87">
+        <v>22.9</v>
+      </c>
+      <c r="C87">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E87">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>2</v>
+      </c>
+      <c r="B88">
+        <v>23</v>
+      </c>
+      <c r="C88">
+        <v>20</v>
+      </c>
+      <c r="E88">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>1.5</v>
+      </c>
+      <c r="B89">
+        <v>23</v>
+      </c>
+      <c r="C89">
+        <v>10.1</v>
+      </c>
+      <c r="E89">
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>1</v>
+      </c>
+      <c r="B90">
+        <v>23.1</v>
+      </c>
+      <c r="C90">
+        <v>10.1</v>
+      </c>
+      <c r="E90">
+        <v>52.7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>0.5</v>
+      </c>
+      <c r="B91">
+        <v>23.2</v>
+      </c>
+      <c r="C91">
+        <v>10.3</v>
+      </c>
+      <c r="E91">
+        <v>52.7</v>
       </c>
     </row>
   </sheetData>
@@ -4067,10 +4920,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3A1FCEB-5AA2-D645-828D-E0266FCEC27F}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A14"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4126,139 +4979,177 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4.5</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="B6">
+        <v>25.3</v>
+      </c>
+      <c r="C6">
+        <v>86</v>
+      </c>
+      <c r="D6">
+        <v>52957</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.72916666666666663</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>25.3</v>
+      </c>
+      <c r="C7">
+        <v>86.6</v>
+      </c>
+      <c r="D7">
+        <v>52966</v>
+      </c>
+      <c r="E7">
+        <v>1.39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>3.5</v>
+        <v>1.5</v>
+      </c>
+      <c r="B8">
+        <v>25.3</v>
+      </c>
+      <c r="C8">
+        <v>91.9</v>
+      </c>
+      <c r="D8">
+        <v>52940</v>
+      </c>
+      <c r="E8">
+        <v>1.33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>25.3</v>
+      </c>
+      <c r="C9">
+        <v>92.6</v>
+      </c>
+      <c r="D9">
+        <v>52930</v>
+      </c>
+      <c r="E9">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="B10">
-        <v>25.3</v>
+        <v>25.2</v>
       </c>
       <c r="C10">
-        <v>86</v>
+        <v>94.9</v>
       </c>
       <c r="D10">
-        <v>52957</v>
+        <v>48300</v>
       </c>
       <c r="E10">
-        <v>4</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.72916666666666663</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>25.3</v>
-      </c>
-      <c r="C11">
-        <v>86.6</v>
-      </c>
-      <c r="D11">
-        <v>52966</v>
-      </c>
-      <c r="E11">
-        <v>1.39</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>1.5</v>
-      </c>
-      <c r="B12">
-        <v>25.3</v>
-      </c>
-      <c r="C12">
-        <v>91.9</v>
-      </c>
-      <c r="D12">
-        <v>52940</v>
-      </c>
-      <c r="E12">
-        <v>1.33</v>
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45282</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>25.3</v>
-      </c>
-      <c r="C13">
-        <v>92.6</v>
-      </c>
-      <c r="D13">
-        <v>52930</v>
-      </c>
-      <c r="E13">
-        <v>1.1000000000000001</v>
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="B14">
-        <v>25.2</v>
+        <v>22.7</v>
       </c>
       <c r="C14">
-        <v>94.9</v>
-      </c>
-      <c r="D14">
-        <v>48300</v>
+        <v>7</v>
       </c>
       <c r="E14">
-        <v>1.3</v>
+        <v>50.2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.52708333333333335</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>22.7</v>
+      </c>
+      <c r="C15">
+        <v>9.02</v>
+      </c>
+      <c r="E15">
+        <v>50.2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1">
-        <v>45282</v>
+      <c r="A16">
+        <v>1.5</v>
+      </c>
+      <c r="B16">
+        <v>22.7</v>
+      </c>
+      <c r="C16">
+        <v>9.08</v>
+      </c>
+      <c r="E16">
+        <v>50.2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" t="s">
-        <v>9</v>
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>22.7</v>
+      </c>
+      <c r="C17">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="E17">
+        <v>50.2</v>
       </c>
       <c r="G17" t="s">
         <v>24</v>
@@ -4266,26 +5157,47 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>4.5</v>
-      </c>
-      <c r="F18" s="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="B18">
+        <v>22.7</v>
+      </c>
+      <c r="C18">
+        <v>9.4</v>
+      </c>
+      <c r="E18">
+        <v>50.1</v>
+      </c>
       <c r="G18">
         <v>4.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>4</v>
-      </c>
-    </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>3.5</v>
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45536</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>3</v>
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -4293,16 +5205,16 @@
         <v>2.5</v>
       </c>
       <c r="B22">
-        <v>22.7</v>
+        <v>24.5</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>8.43</v>
       </c>
       <c r="E22">
-        <v>50.2</v>
+        <v>50.9</v>
       </c>
       <c r="F22" s="2">
-        <v>0.52708333333333335</v>
+        <v>0.53472222222222221</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -4310,13 +5222,13 @@
         <v>2</v>
       </c>
       <c r="B23">
-        <v>22.7</v>
+        <v>24.5</v>
       </c>
       <c r="C23">
-        <v>9.02</v>
+        <v>8.5</v>
       </c>
       <c r="E23">
-        <v>50.2</v>
+        <v>50.8</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -4324,13 +5236,16 @@
         <v>1.5</v>
       </c>
       <c r="B24">
-        <v>22.7</v>
+        <v>24.5</v>
       </c>
       <c r="C24">
-        <v>9.08</v>
+        <v>8.76</v>
       </c>
       <c r="E24">
-        <v>50.2</v>
+        <v>50.7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -4338,13 +5253,16 @@
         <v>1</v>
       </c>
       <c r="B25">
-        <v>22.7</v>
+        <v>24.5</v>
       </c>
       <c r="C25">
-        <v>9.1199999999999992</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="E25">
-        <v>50.2</v>
+        <v>50.7</v>
+      </c>
+      <c r="G25">
+        <v>4.5</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -4352,21 +5270,21 @@
         <v>0.5</v>
       </c>
       <c r="B26">
-        <v>22.7</v>
+        <v>24.5</v>
       </c>
       <c r="C26">
-        <v>9.4</v>
+        <v>9.0299999999999994</v>
       </c>
       <c r="E26">
-        <v>50.1</v>
+        <v>50.7</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="1">
-        <v>45536</v>
+      <c r="B28" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -4394,99 +5312,185 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>4.5</v>
-      </c>
-      <c r="F30" s="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="B30">
+        <v>25.3</v>
+      </c>
+      <c r="C30">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="E30">
+        <v>51.2</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.5</v>
+      </c>
       <c r="G30">
-        <v>4.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>25.3</v>
+      </c>
+      <c r="C31">
+        <v>8.52</v>
+      </c>
+      <c r="E31">
+        <v>51.2</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.5</v>
+      </c>
+      <c r="B32">
+        <v>25.3</v>
+      </c>
+      <c r="C32">
+        <v>9.08</v>
+      </c>
+      <c r="E32">
+        <v>51.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>25.6</v>
+      </c>
+      <c r="C33">
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="E33">
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="B34">
-        <v>24.5</v>
+        <v>25.5</v>
       </c>
       <c r="C34">
-        <v>8.43</v>
+        <v>9.4</v>
       </c>
       <c r="E34">
         <v>50.9</v>
       </c>
-      <c r="F34" s="2">
-        <v>0.53472222222222221</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>2</v>
-      </c>
-      <c r="B35">
-        <v>24.5</v>
-      </c>
-      <c r="C35">
-        <v>8.5</v>
-      </c>
-      <c r="E35">
-        <v>50.8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2.5</v>
+      </c>
+      <c r="B38">
+        <v>23.3</v>
+      </c>
+      <c r="C38">
+        <v>10.3</v>
+      </c>
+      <c r="E38">
+        <v>52.3</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="G38">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>23.4</v>
+      </c>
+      <c r="C39">
+        <v>10.3</v>
+      </c>
+      <c r="E39">
+        <v>52.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>1.5</v>
       </c>
-      <c r="B36">
-        <v>24.5</v>
-      </c>
-      <c r="C36">
-        <v>8.76</v>
-      </c>
-      <c r="E36">
-        <v>50.7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37">
-        <v>24.5</v>
-      </c>
-      <c r="C37">
-        <v>8.9700000000000006</v>
-      </c>
-      <c r="E37">
-        <v>50.7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="B40">
+        <v>23.4</v>
+      </c>
+      <c r="C40">
+        <v>10.1</v>
+      </c>
+      <c r="E40">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>23.8</v>
+      </c>
+      <c r="C41">
+        <v>10.1</v>
+      </c>
+      <c r="E41">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
         <v>0.5</v>
       </c>
-      <c r="B38">
-        <v>24.5</v>
-      </c>
-      <c r="C38">
-        <v>9.0299999999999994</v>
-      </c>
-      <c r="E38">
-        <v>50.7</v>
+      <c r="B42">
+        <v>23.9</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="E42">
+        <v>52.2</v>
       </c>
     </row>
   </sheetData>
@@ -4499,7 +5503,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4555,268 +5559,278 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4.5</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>24.7</v>
+      </c>
+      <c r="C6">
+        <v>101</v>
+      </c>
+      <c r="D6">
+        <v>50313</v>
+      </c>
+      <c r="E6">
+        <v>1.23</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.74305555555555547</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>3.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="B7">
+        <v>24.7</v>
+      </c>
+      <c r="C7">
+        <v>100.7</v>
+      </c>
+      <c r="D7">
+        <v>50000</v>
+      </c>
+      <c r="E7">
+        <v>1.17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>3</v>
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45282</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>2.5</v>
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>22.9</v>
+      </c>
+      <c r="C11">
+        <v>11.99</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.53263888888888888</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>24.7</v>
-      </c>
-      <c r="C13">
-        <v>101</v>
-      </c>
-      <c r="D13">
-        <v>50313</v>
-      </c>
-      <c r="E13">
-        <v>1.23</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0.74305555555555547</v>
+        <v>0.5</v>
+      </c>
+      <c r="B12">
+        <v>22.9</v>
+      </c>
+      <c r="C12">
+        <v>9.85</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45536</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>24.5</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>50.8</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.54861111111111105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>0.5</v>
       </c>
-      <c r="B14">
-        <v>24.7</v>
-      </c>
-      <c r="C14">
-        <v>100.7</v>
-      </c>
-      <c r="D14">
-        <v>50000</v>
-      </c>
-      <c r="E14">
-        <v>1.17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1">
-        <v>45282</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17">
+        <v>24.5</v>
+      </c>
+      <c r="C17">
+        <v>9.09</v>
+      </c>
+      <c r="E17">
+        <v>50.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
         <v>6</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D20" t="s">
         <v>7</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E20" t="s">
         <v>22</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F20" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>4.5</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>3.5</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>25.3</v>
+      </c>
+      <c r="C21">
+        <v>8.9</v>
+      </c>
+      <c r="E21">
+        <v>51.1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.50694444444444442</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>2</v>
+        <v>0.5</v>
+      </c>
+      <c r="B22">
+        <v>25.3</v>
+      </c>
+      <c r="C22">
+        <v>9.48</v>
+      </c>
+      <c r="E22">
+        <v>50.9</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>1.5</v>
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25">
-        <v>22.9</v>
-      </c>
-      <c r="C25">
-        <v>11.99</v>
-      </c>
-      <c r="E25">
-        <v>50</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0.53263888888888888</v>
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>23.8</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>52</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.62152777777777779</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>0.5</v>
       </c>
-      <c r="B26">
-        <v>22.9</v>
-      </c>
-      <c r="C26">
-        <v>9.85</v>
-      </c>
-      <c r="E26">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="1">
-        <v>45536</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>4.5</v>
-      </c>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37">
-        <v>24.5</v>
-      </c>
-      <c r="C37">
-        <v>9</v>
-      </c>
-      <c r="E37">
-        <v>50.8</v>
-      </c>
-      <c r="F37" s="2">
-        <v>0.54861111111111105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>0.5</v>
-      </c>
-      <c r="B38">
-        <v>24.5</v>
-      </c>
-      <c r="C38">
-        <v>9.09</v>
-      </c>
-      <c r="E38">
-        <v>50.7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>24</v>
+      </c>
+      <c r="C27">
+        <v>10.3</v>
+      </c>
+      <c r="E27">
+        <v>52.9</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.2">
       <c r="H39" t="s">
         <v>26</v>
       </c>
@@ -4830,7 +5844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DBE86B5-8884-DF4C-A32B-B830DCC4A392}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>